<commit_message>
Actualizar documentos de modelo enriquecido
</commit_message>
<xml_diff>
--- a/ModelosEnriquecidos/Modelo enriquecido - Accesos.xlsx
+++ b/ModelosEnriquecidos/Modelo enriquecido - Accesos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\archivos\Downloads\modelos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Información\Downloads\DOO-working-group\ModelosEnriquecidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31C0283-61F8-4900-84E6-E738486B4E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46928AAC-A639-4C89-800A-6E84855243C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="2" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="3" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de dominio anémico" sheetId="61" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="78">
   <si>
     <t>Descripción</t>
   </si>
@@ -235,23 +235,57 @@
     <t>Es la fecha en la que se crea un acceso de un usuario a un equipo de trabajo</t>
   </si>
   <si>
-    <t>Unico</t>
-  </si>
-  <si>
-    <t>Atributo que es unico y no se debe repetir en ningun otro atributo</t>
-  </si>
-  <si>
     <t>Es el identificador unico del objeto IngresarIntegrante el cual esta en el formato especial UUID</t>
   </si>
   <si>
     <t>Es el identificador unico del objeto EnviarCorreo el cual esta en el formato especial UUID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>AccesoRelacionado</t>
+  </si>
+  <si>
+    <t>CorreoDestino</t>
+  </si>
+  <si>
+    <t>Correo electronico valido, iniciado por una serie de caracteres junto con @ y seguido de un dominio</t>
+  </si>
+  <si>
+    <t>Corresponde a una cadena de caracteres conformada por [A-Z][a-z][0-9]
+@ y caracteres especiales</t>
+  </si>
+  <si>
+    <t>Es el correo electronico al cual se envia la notificación</t>
+  </si>
+  <si>
+    <t>NotificacionRelacionada</t>
+  </si>
+  <si>
+    <t>Notificación (Notificaciones)</t>
+  </si>
+  <si>
+    <t>Formato de nombre de un equipo valido traido de Accesos</t>
+  </si>
+  <si>
+    <t>Corresponde a una cadena de caracteres conformada por[A-Z][a-z][0-9]</t>
+  </si>
+  <si>
+    <t>Es el nombre del equipo del cual se desea enviar su notificación de acceso</t>
+  </si>
+  <si>
+    <t>IdUsuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,8 +333,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,6 +402,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -533,7 +580,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -689,6 +736,12 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -766,9 +819,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -799,23 +849,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>324970</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>67235</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>78441</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>334495</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>162485</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>87966</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>29696</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C68679BF-844D-F9E1-97A9-F3A3437B55EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CF42AF2-C34B-CEF7-059C-92FAF01594FE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -838,8 +888,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7944970" y="2924735"/>
-          <a:ext cx="3819525" cy="2381250"/>
+          <a:off x="9222441" y="3372971"/>
+          <a:ext cx="3819525" cy="2752725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1158,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFF4C49-240B-4036-BD62-669D42F23E67}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="W29" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,6 +1224,9 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H9"/>
+    </row>
+    <row r="20" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R20"/>
     </row>
     <row r="35" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N35"/>
@@ -1272,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235BA608-57CC-45B0-8234-10CA49C3B004}">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView zoomScale="104" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,70 +1357,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="54" t="str">
+      <c r="B2" s="56" t="str">
         <f>'Listado Objetos de Dominio'!$A$2</f>
         <v>Acceso</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55" t="str">
+      <c r="B3" s="57" t="str">
         <f>'Listado Objetos de Dominio'!$B$2</f>
         <v>Objeto de dominio que representa cada acceso de un usuario hacia un equipo de trabajo</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1419,19 +1472,19 @@
         <v>0</v>
       </c>
       <c r="Q4" s="37" t="str">
-        <f>A16</f>
+        <f>A18</f>
         <v>Reponsabilidad 1</v>
       </c>
       <c r="R4" s="35" t="str">
-        <f>A17</f>
+        <f>A19</f>
         <v>Reponsabilidad 2</v>
       </c>
       <c r="S4" s="36" t="str">
-        <f>A18</f>
+        <f>A20</f>
         <v>Reponsabilidad 3</v>
       </c>
       <c r="T4" s="2" t="str">
-        <f>A19</f>
+        <f>A21</f>
         <v>Reponsabilidad 4</v>
       </c>
     </row>
@@ -1527,7 +1580,7 @@
       <c r="A7" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="53" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="5"/>
@@ -1553,7 +1606,7 @@
       <c r="A8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="79" t="s">
+      <c r="B8" s="53" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="5"/>
@@ -1575,233 +1628,319 @@
       <c r="S8" s="28"/>
       <c r="T8" s="31"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+    <row r="9" spans="1:20" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="5">
+        <v>32</v>
+      </c>
+      <c r="D9" s="5">
+        <v>32</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="5"/>
+      <c r="J9" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="31"/>
+    </row>
+    <row r="10" spans="1:20" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="5">
+        <v>32</v>
+      </c>
+      <c r="D10" s="5">
+        <v>32</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="31"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B13" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C13" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+    <row r="14" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="38"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60" t="s">
+      <c r="B16" s="62"/>
+      <c r="C16" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60" t="s">
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60" t="s">
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60" t="s">
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60" t="s">
+      <c r="P16" s="62"/>
+      <c r="Q16" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="R14" s="63"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="19" t="s">
+      <c r="R16" s="65"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="63"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H17" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I17" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J17" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="62" t="s">
+      <c r="K17" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62"/>
-      <c r="O15" s="19" t="s">
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="P15" s="19" t="s">
+      <c r="P17" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="Q15" s="19" t="s">
+      <c r="Q17" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="R15" s="25" t="s">
+      <c r="R17" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="26"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
+      <c r="B18" s="67"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="26"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="27"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="72" t="s">
+      <c r="B19" s="79"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="73"/>
+      <c r="N19" s="73"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="27"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="29"/>
-      <c r="R18" s="30"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="68" t="s">
+      <c r="B20" s="75"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
+      <c r="M20" s="77"/>
+      <c r="N20" s="77"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="30"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="67"/>
-      <c r="N19" s="67"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="33"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:F21"/>
     <mergeCell ref="K19:N19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="K20:N20"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:F19"/>
+    <mergeCell ref="Q16:R16"/>
     <mergeCell ref="K17:N17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="K18:N18"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="K16:N16"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B3:P3"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:F15"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="C16:F17"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:N16"/>
+    <mergeCell ref="O16:P16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{F92E8141-0BAA-4CFF-A2AA-790349ADA214}"/>
-    <hyperlink ref="H19" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{9CFC97C1-FDC7-4BCC-A442-03CBBA306898}"/>
+    <hyperlink ref="H21" location="'Tipo Relación Institución'!A6" display="'Tipo Relación Institución'!A6" xr:uid="{9CFC97C1-FDC7-4BCC-A442-03CBBA306898}"/>
     <hyperlink ref="R4" location="'Objeto Dominio 2'!A17" display="'Objeto Dominio 2'!A17" xr:uid="{C31578C6-097C-48B5-85BE-E2B5695507BB}"/>
     <hyperlink ref="S4" location="'Objeto Dominio 2'!A18" display="'Objeto Dominio 2'!A18" xr:uid="{12E63051-0357-4C9D-ABE2-AAC9F4D1077D}"/>
     <hyperlink ref="T4" location="'Objeto Dominio 2'!A19" display="'Objeto Dominio 2'!A19" xr:uid="{1EEF2DB2-A99F-4C59-8304-4835FA7407E0}"/>
-    <hyperlink ref="A17:B17" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{821E0C47-3835-4659-B0FA-56687A0DE151}"/>
-    <hyperlink ref="A16:B16" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{22905DC7-C781-450C-BA99-3B5AF5CDD56E}"/>
-    <hyperlink ref="A19:B19" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{98480B8D-5789-4D0D-9A12-1FCE9FA5B81E}"/>
+    <hyperlink ref="A19:B19" location="'Objeto Dominio 2'!R4" display="Reponsabilidad 2" xr:uid="{821E0C47-3835-4659-B0FA-56687A0DE151}"/>
+    <hyperlink ref="A18:B18" location="'Objeto Dominio 2'!Q4" display="Reponsabilidad 1" xr:uid="{22905DC7-C781-450C-BA99-3B5AF5CDD56E}"/>
+    <hyperlink ref="A21:B21" location="'Objeto Dominio 2'!T4" display="Reponsabilidad 4" xr:uid="{98480B8D-5789-4D0D-9A12-1FCE9FA5B81E}"/>
     <hyperlink ref="Q4" location="'Objeto Dominio 2'!A16" display="'Objeto Dominio 2'!A16" xr:uid="{F66CECC3-2EE1-49F8-9E57-39E041254432}"/>
     <hyperlink ref="A1:P1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{BAD90D86-7311-49B0-A802-02D69BE204D5}"/>
-    <hyperlink ref="A18:B18" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{1BF344DA-00DC-4E3D-9686-31B0C99A39F5}"/>
-    <hyperlink ref="B8" location="'Objeto Dominio IngresarIntegran'!A1" display="IngresarIntegrante" xr:uid="{4FD8F2F6-C53C-4D10-90F8-9F27A721FCCB}"/>
+    <hyperlink ref="A20:B20" location="'Objeto Dominio 2'!S4" display="Reponsabilidad 3" xr:uid="{1BF344DA-00DC-4E3D-9686-31B0C99A39F5}"/>
     <hyperlink ref="B7" location="'Objeto Dominio EnviarCorreo'!A1" display="EnviarCorreo" xr:uid="{4204E4FE-A3A6-4083-9974-30F7685579D9}"/>
+    <hyperlink ref="B8" location="'Objeto Dominio IngresarIntegran'!A1" display="IngresarIntegrante" xr:uid="{B18A4079-B887-480A-8ECC-6C74644B2471}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1812,7 +1951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9732BFC6-5B3A-4E40-BEA3-58E7EDB79B0C}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
     </sheetView>
@@ -1844,70 +1983,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="54" t="str">
+      <c r="B2" s="56" t="str">
         <f>'Listado Objetos de Dominio'!$A$3</f>
         <v>IngresarIntegrante</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55" t="str">
+      <c r="B3" s="57" t="str">
         <f>'Listado Objetos de Dominio'!$B$3</f>
         <v>Objeto de dominio que contiene el ingreso de un integrante en un equipo de trabajo</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2014,7 +2153,7 @@
         <v>44</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q5" s="34"/>
       <c r="R5" s="23"/>
@@ -2089,11 +2228,11 @@
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="60"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
@@ -2112,44 +2251,44 @@
       <c r="C12" s="38"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60" t="s">
+      <c r="B14" s="62"/>
+      <c r="C14" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60" t="s">
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60" t="s">
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60" t="s">
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60" t="s">
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="R14" s="63"/>
+      <c r="R14" s="65"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
       <c r="G15" s="19" t="s">
         <v>28</v>
       </c>
@@ -2162,12 +2301,12 @@
       <c r="J15" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="62" t="s">
+      <c r="K15" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
       <c r="O15" s="19" t="s">
         <v>30</v>
       </c>
@@ -2182,88 +2321,88 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
       <c r="G16" s="20"/>
       <c r="H16" s="21"/>
       <c r="I16" s="22"/>
       <c r="J16" s="21"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
       <c r="R16" s="26"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
       <c r="G17" s="46"/>
       <c r="H17" s="44"/>
       <c r="I17" s="45"/>
       <c r="J17" s="39"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
       <c r="O17" s="23"/>
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
       <c r="R17" s="27"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
       <c r="G18" s="42"/>
       <c r="H18" s="40"/>
       <c r="I18" s="41"/>
       <c r="J18" s="43"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
+      <c r="K18" s="77"/>
+      <c r="L18" s="77"/>
+      <c r="M18" s="77"/>
+      <c r="N18" s="77"/>
       <c r="O18" s="28"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="29"/>
       <c r="R18" s="30"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
       <c r="G19" s="48"/>
       <c r="H19" s="49"/>
       <c r="I19" s="47"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="67"/>
-      <c r="N19" s="67"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
       <c r="O19" s="31"/>
       <c r="P19" s="32"/>
       <c r="Q19" s="32"/>
@@ -2317,7 +2456,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2347,70 +2486,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="A1" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="54" t="str">
+      <c r="B2" s="56" t="str">
         <f>'Listado Objetos de Dominio'!$A$4</f>
         <v>EnviarCorreo</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="55" t="str">
+      <c r="B3" s="57" t="str">
         <f>'Listado Objetos de Dominio'!$B$4</f>
         <v>Objeto de dominio que representa la notificación de ser agregado a un equipo de trabajo</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -2517,60 +2656,112 @@
         <v>44</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q5" s="34"/>
       <c r="R5" s="23"/>
       <c r="S5" s="28"/>
       <c r="T5" s="31"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+    <row r="6" spans="1:20" ht="51" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="5">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5">
+        <v>32</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="I6" s="5"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="7"/>
+      <c r="J6" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" s="54" t="s">
+        <v>76</v>
+      </c>
       <c r="Q6" s="34"/>
       <c r="R6" s="23"/>
       <c r="S6" s="28"/>
       <c r="T6" s="31"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+    <row r="7" spans="1:20" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>100</v>
+      </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="H7" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="7"/>
+      <c r="J7" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="Q7" s="34"/>
       <c r="R7" s="23"/>
       <c r="S7" s="28"/>
       <c r="T7" s="31"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="5"/>
+    <row r="8" spans="1:20" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -2592,11 +2783,11 @@
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="58"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="60"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
@@ -2613,47 +2804,50 @@
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
       <c r="C12" s="38"/>
+      <c r="D12" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60" t="s">
+      <c r="B14" s="62"/>
+      <c r="C14" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60" t="s">
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60" t="s">
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60" t="s">
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60" t="s">
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="R14" s="63"/>
+      <c r="R14" s="65"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
       <c r="G15" s="19" t="s">
         <v>28</v>
       </c>
@@ -2666,12 +2860,12 @@
       <c r="J15" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="62" t="s">
+      <c r="K15" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
-      <c r="N15" s="62"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
       <c r="O15" s="19" t="s">
         <v>30</v>
       </c>
@@ -2686,88 +2880,88 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
       <c r="G16" s="20"/>
       <c r="H16" s="21"/>
       <c r="I16" s="22"/>
       <c r="J16" s="21"/>
-      <c r="K16" s="66"/>
-      <c r="L16" s="66"/>
-      <c r="M16" s="66"/>
-      <c r="N16" s="66"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
       <c r="R16" s="26"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
       <c r="G17" s="46"/>
       <c r="H17" s="44"/>
       <c r="I17" s="45"/>
       <c r="J17" s="39"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
       <c r="O17" s="23"/>
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
       <c r="R17" s="27"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
       <c r="G18" s="42"/>
       <c r="H18" s="40"/>
       <c r="I18" s="41"/>
       <c r="J18" s="43"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
+      <c r="K18" s="77"/>
+      <c r="L18" s="77"/>
+      <c r="M18" s="77"/>
+      <c r="N18" s="77"/>
       <c r="O18" s="28"/>
       <c r="P18" s="29"/>
       <c r="Q18" s="29"/>
       <c r="R18" s="30"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
       <c r="G19" s="48"/>
       <c r="H19" s="49"/>
       <c r="I19" s="47"/>
       <c r="J19" s="48"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="67"/>
-      <c r="N19" s="67"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
       <c r="O19" s="31"/>
       <c r="P19" s="32"/>
       <c r="Q19" s="32"/>

</xml_diff>